<commit_message>
Atualização automática de CACHOEIRA_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/CACHOEIRA_DO_SUL.xlsx
+++ b/CACHOEIRA_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1BEB966-B267-4F05-8840-91D250F9D1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C31BFCEE-9D38-4E3B-8021-8002482BEC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1208,7 +1195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1268,36 +1255,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1336,14 +1299,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1395,7 +1353,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{80A6EE9C-293C-4661-8BFE-2B56C83C35F4}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{19E8619E-C8A8-40BE-8143-7AFBDA2F9A46}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1425,10 +1383,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6AE776-1029-4788-BA1D-8BCA2FCEA78F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB768365-47A9-49DC-A743-F07A2BA2DA7F}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1466,7 +1424,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36740CB7-082D-49C6-9C16-FC1AE07E3AE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD77F498-12D7-4A22-B1F9-D60A57BE790B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1529,7 +1487,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE93BE8D-0088-43BD-94B8-8D6B37D59F1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD0C5441-64D3-4628-B701-64A7F94D7387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1548,7 +1506,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C1A606-4BBA-41A5-5030-58BA54E4D19E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8347E09E-30EB-0AF9-1BBE-306B8500978A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1597,7 +1555,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E4DD7FF-D84A-8068-0FA6-1487B58C0E5F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6117EED-E125-76C5-4DA6-A79A3BD6D34E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1616,7 +1574,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3375D9BE-9C37-F9CF-B39B-6AE13C4A2F0B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{981BE73F-D417-F561-039B-1B809C9DC90C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1647,7 +1605,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A75CD0C0-973E-9A70-893C-DDEFE4AA27FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48A99CC6-98E2-93C7-31F8-7D1E8678DA2A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1678,7 +1636,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBFDF08A-797D-38B1-8BB8-A4C04C7B112F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4FA3FF4-8B79-2189-4360-687F73FD2788}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1721,7 +1679,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A1362A-6FB2-4C91-B259-24DBD165F048}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A321F66-AF4E-41EE-9834-CF2DAD6AAA3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1759,7 +1717,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC50B3F-E0E9-4D11-AAD9-2E20C4D75D96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DCA5A84-E00E-4EA1-BD90-EC01D0315252}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1802,7 +1760,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24780B58-9ABE-4E94-BFCC-997E75AE6AEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{176EBF3A-78F9-4785-A3DD-6202C33B1A49}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2115,7 +2073,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF1D118-63B2-4974-A44A-B65292AD2369}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CA9C49-E595-43AD-B741-547DCFE399E3}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2127,98 +2085,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="39"/>
-    <col min="6" max="6" width="2" style="39" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="39" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="39"/>
+    <col min="1" max="5" width="12.5703125" style="36"/>
+    <col min="6" max="6" width="2" style="36" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="38"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="38"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="38"/>
+      <c r="F3" s="35"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="38"/>
+      <c r="F4" s="35"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="38"/>
+      <c r="F5" s="35"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="38"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="38"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="38"/>
+      <c r="F8" s="35"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="38"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="38"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="38"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="38"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="38"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="38"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="38"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="38"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="38"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="38"/>
+      <c r="F18" s="35"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="38"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="38"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="38"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="38"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="38"/>
+      <c r="F23" s="35"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="38"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="38"/>
+      <c r="F25" s="35"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="38"/>
+      <c r="F26" s="35"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="38"/>
+      <c r="F27" s="35"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="38"/>
+      <c r="F28" s="35"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="38"/>
+      <c r="F29" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5484,19 +5442,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>272</v>
       </c>
     </row>
@@ -5519,90 +5477,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>278</v>
       </c>
     </row>
@@ -5620,16 +5578,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5663,7 +5621,7 @@
       <c r="J1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5677,10 +5635,10 @@
       <c r="C2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="21">
         <v>310</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="21">
         <v>31</v>
       </c>
       <c r="F2" s="2">
@@ -5698,7 +5656,7 @@
       <c r="J2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="22">
         <v>10010</v>
       </c>
     </row>
@@ -5712,10 +5670,10 @@
       <c r="C3" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="21">
         <v>140</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="21">
         <v>14</v>
       </c>
       <c r="F3" s="2">
@@ -5733,7 +5691,7 @@
       <c r="J3" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="K3" s="25">
+      <c r="K3" s="22">
         <v>9363</v>
       </c>
     </row>
@@ -5747,10 +5705,10 @@
       <c r="C4" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="21">
         <v>106</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="21">
         <v>10.6</v>
       </c>
       <c r="F4" s="2">
@@ -5768,7 +5726,7 @@
       <c r="J4" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K4" s="25">
+      <c r="K4" s="22">
         <v>1085</v>
       </c>
     </row>
@@ -5782,10 +5740,10 @@
       <c r="C5" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="21">
         <v>144</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="21">
         <v>14.4</v>
       </c>
       <c r="F5" s="2">
@@ -5803,7 +5761,7 @@
       <c r="J5" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="22">
         <v>658</v>
       </c>
     </row>
@@ -5817,10 +5775,10 @@
       <c r="C6" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <v>263</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="21">
         <v>26.3</v>
       </c>
       <c r="F6" s="2">
@@ -5838,7 +5796,7 @@
       <c r="J6" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="22">
         <v>9363</v>
       </c>
     </row>
@@ -5852,10 +5810,10 @@
       <c r="C7" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <v>287</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="21">
         <v>28.7</v>
       </c>
       <c r="F7" s="2">
@@ -5873,7 +5831,7 @@
       <c r="J7" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -5887,10 +5845,10 @@
       <c r="C8" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <v>800</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>80</v>
       </c>
       <c r="F8" s="2">
@@ -5908,7 +5866,7 @@
       <c r="J8" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <v>275</v>
       </c>
     </row>
@@ -5922,10 +5880,10 @@
       <c r="C9" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>480.1</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>48.01</v>
       </c>
       <c r="F9" s="2">
@@ -5943,7 +5901,7 @@
       <c r="J9" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <v>656</v>
       </c>
     </row>
@@ -5957,10 +5915,10 @@
       <c r="C10" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>480.1</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <v>48.01</v>
       </c>
       <c r="F10" s="2">
@@ -5978,7 +5936,7 @@
       <c r="J10" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -5992,10 +5950,10 @@
       <c r="C11" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>480.1</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <v>48.01</v>
       </c>
       <c r="F11" s="2">
@@ -6013,7 +5971,7 @@
       <c r="J11" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -6027,10 +5985,10 @@
       <c r="C12" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="21">
         <v>480.1</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="21">
         <v>48.01</v>
       </c>
       <c r="F12" s="2">
@@ -6048,7 +6006,7 @@
       <c r="J12" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -6062,10 +6020,10 @@
       <c r="C13" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="21">
         <v>480.1</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="21">
         <v>48.01</v>
       </c>
       <c r="F13" s="2">
@@ -6083,7 +6041,7 @@
       <c r="J13" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -6097,10 +6055,10 @@
       <c r="C14" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="21">
         <v>480.1</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="21">
         <v>48.01</v>
       </c>
       <c r="F14" s="2">
@@ -6118,7 +6076,7 @@
       <c r="J14" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -6132,10 +6090,10 @@
       <c r="C15" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <v>480.1</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="21">
         <v>48.01</v>
       </c>
       <c r="F15" s="2">
@@ -6153,7 +6111,7 @@
       <c r="J15" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="22">
         <v>11772</v>
       </c>
     </row>
@@ -6167,10 +6125,10 @@
       <c r="C16" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>127.05</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>12.71</v>
       </c>
       <c r="F16" s="2">
@@ -6188,7 +6146,7 @@
       <c r="J16" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="22">
         <v>275</v>
       </c>
     </row>
@@ -6202,10 +6160,10 @@
       <c r="C17" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="21">
         <v>448</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <v>44.8</v>
       </c>
       <c r="F17" s="2">
@@ -6223,7 +6181,7 @@
       <c r="J17" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="22">
         <v>11772</v>
       </c>
     </row>
@@ -6237,10 +6195,10 @@
       <c r="C18" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>134</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>13.4</v>
       </c>
       <c r="F18" s="2">
@@ -6258,7 +6216,7 @@
       <c r="J18" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="22">
         <v>11772</v>
       </c>
     </row>
@@ -6272,10 +6230,10 @@
       <c r="C19" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="21">
         <v>500</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="21">
         <v>50</v>
       </c>
       <c r="F19" s="2">
@@ -6293,7 +6251,7 @@
       <c r="J19" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="22">
         <v>656</v>
       </c>
     </row>
@@ -6307,10 +6265,10 @@
       <c r="C20" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="21">
         <v>1954</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="21">
         <v>195.4</v>
       </c>
       <c r="F20" s="2">
@@ -6328,7 +6286,7 @@
       <c r="J20" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="22">
         <v>275</v>
       </c>
     </row>
@@ -6342,10 +6300,10 @@
       <c r="C21" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="21">
         <v>360</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="21">
         <v>36</v>
       </c>
       <c r="F21" s="2">
@@ -6363,7 +6321,7 @@
       <c r="J21" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K21" s="25">
+      <c r="K21" s="22">
         <v>275</v>
       </c>
     </row>
@@ -6377,10 +6335,10 @@
       <c r="C22" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="21">
         <v>221</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="21">
         <v>22.1</v>
       </c>
       <c r="F22" s="2">
@@ -6398,7 +6356,7 @@
       <c r="J22" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K22" s="25">
+      <c r="K22" s="22">
         <v>972</v>
       </c>
     </row>
@@ -6412,10 +6370,10 @@
       <c r="C23" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="21">
         <v>164.15</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="21">
         <v>16.420000000000002</v>
       </c>
       <c r="F23" s="2">
@@ -6433,7 +6391,7 @@
       <c r="J23" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="22">
         <v>656</v>
       </c>
     </row>
@@ -6447,10 +6405,10 @@
       <c r="C24" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="21">
         <v>402.08</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="21">
         <v>40.21</v>
       </c>
       <c r="F24" s="2">
@@ -6468,7 +6426,7 @@
       <c r="J24" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="22">
         <v>656</v>
       </c>
     </row>
@@ -6482,10 +6440,10 @@
       <c r="C25" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="21">
         <v>790</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="21">
         <v>79</v>
       </c>
       <c r="F25" s="2">
@@ -6503,7 +6461,7 @@
       <c r="J25" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="22">
         <v>656</v>
       </c>
     </row>
@@ -6517,10 +6475,10 @@
       <c r="C26" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="21">
         <v>2113.4</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="21">
         <v>422.68</v>
       </c>
       <c r="F26" s="2">
@@ -6538,7 +6496,7 @@
       <c r="J26" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="22">
         <v>275</v>
       </c>
     </row>
@@ -6552,10 +6510,10 @@
       <c r="C27" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="21">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <v>999.73</v>
       </c>
       <c r="F27" s="2">
@@ -6573,7 +6531,7 @@
       <c r="J27" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="22">
         <v>12273</v>
       </c>
     </row>
@@ -6598,54 +6556,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="23" t="s">
         <v>336</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>339</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>341</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>342</v>
       </c>
     </row>
@@ -6656,43 +6615,43 @@
       <c r="B2" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="26">
         <v>45748</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="27">
         <v>5658</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="27" t="s">
         <v>344</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>54254</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>4276</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="29" t="s">
         <v>345</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="29" t="s">
         <v>345</v>
       </c>
     </row>
@@ -6723,25 +6682,24 @@
       <c r="B1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="E1" s="34">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="31">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="34">
         <v>69</v>
       </c>
-      <c r="F1" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>294</v>
-      </c>
-      <c r="B2" s="37">
-        <v>69</v>
-      </c>
-      <c r="C2" s="35">
+      <c r="C2" s="32">
         <v>4.5628885068112676E-3</v>
       </c>
     </row>

</xml_diff>